<commit_message>
feat:update dragon location excel
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>int</t>
   </si>
@@ -116,22 +116,43 @@
     <t>Cowlevel001</t>
   </si>
   <si>
-    <t>506276.25|-15371|1068||506276.25|42784.48|46083.01||495329.25|43252.48|46083.01||497870.25|53525.48|46083.01||497870.25|53525.48|49234.01||503903.25|53525.48|49234.01||504647.25|47997.48|49003.01||499929.25|47997.48|49003.01</t>
+    <t>506276.25|42784.48|46083.01||495329.25|43252.48|46083.01||497870.25|53525.48|46083.01||497870.25|53525.48|47007||503903.25|53525.48|47007||504647.25|47997.48|47007||499929.25|47997.48|47007</t>
   </si>
   <si>
     <t>Cowlevel002</t>
   </si>
   <si>
+    <t>598563.75|594154.88|7143.97||602921.75|595009.88|7143.97||602921.75|595009.88|7851.97||602921.75|601241.88|7851.97||598241.75|602673.88|7851.97||598241.75|594819.88|7851.97||602921.75|600363.88|7295.97</t>
+  </si>
+  <si>
     <t>Cowlevel003</t>
   </si>
   <si>
+    <t>498910.44|46868.74|45986||496482.44|48743.74|45986||498294.44|55570.74|45986||499992.44|56135.74|45986||499992.44|56135.74|46753.00||499228.44|47348.74|46753||496626.44|48303.74|46753||498189.44|55497.74|46424</t>
+  </si>
+  <si>
     <t>Cowlevel004</t>
   </si>
   <si>
+    <t>97705.11|1001785.63|6204.8||97705.11|995826.63|6204.8||101330.11|995826.63|6204.8||101330.11|1001359.63|6204.80||101330.11|1001359.63|6911.80||97885.11|1001359.63|6911.80||97885.11|996353.63|6911.80||101778.11|996223.63|6911.80</t>
+  </si>
+  <si>
     <t>Cowlevel005</t>
   </si>
   <si>
+    <t>98879.05|1000148.06|10082||98879.05|997982.06|10082||100784.05|997982.06|10082||100186.05|999942.06|10082||99185.45|999750.75|10589||99239.05|998549.06|10590||99851.05|998549.06|10590||99851.05|999709.06|10590</t>
+  </si>
+  <si>
     <t>Cowlevel006</t>
+  </si>
+  <si>
+    <t>1010497.13|18739.56|4593.87||1006911.13|16723.56|4593.87||1004790.13|19763.56|4593.87||1006629.13|19763.56|5473.87||1009839.13|18905.56|5473.87||1007139.13|17599.56|5473.87</t>
+  </si>
+  <si>
+    <t>Cowlevel007</t>
+  </si>
+  <si>
+    <t>8978.4|229.39|296699.97||5201.4|229.39|296699.97||5201.4|5546.39|296699.97||6494.4|5546.39|296699.97||6494.4|5037.39|297305.97||6494.4|1696.39|297305.97||5428.4|3174.39|297305.97</t>
   </si>
 </sst>
 </file>
@@ -144,7 +165,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -153,12 +174,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
@@ -617,148 +632,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -776,10 +791,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1052,7 +1067,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{3A8F5873-6032-4FB4-99FC-23539F5AA27B}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{8E19E395-D54C-409B-98D3-2393F0804047}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1061,7 +1076,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{03C3174D-61CA-4D0A-9CF9-C6C99977A597}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{E14272A0-B37D-4031-840A-CD97D57AD41B}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1294,8 +1309,8 @@
   <sheetPr/>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" outlineLevelCol="5"/>
@@ -1518,7 +1533,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" s="2" customFormat="1" ht="49.5" spans="1:6">
+    <row r="19" s="2" customFormat="1" ht="33" spans="1:6">
       <c r="A19" s="8">
         <v>15</v>
       </c>
@@ -1532,49 +1547,71 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" s="2" customFormat="1" spans="1:2">
+    <row r="20" s="2" customFormat="1" spans="1:3">
       <c r="A20" s="8">
         <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" s="2" customFormat="1" spans="1:2">
+      <c r="C20" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" spans="1:3">
       <c r="A21" s="8">
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" s="2" customFormat="1" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" spans="1:3">
       <c r="A22" s="8">
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" s="2" customFormat="1" spans="1:2">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" s="2" customFormat="1" spans="1:3">
       <c r="A23" s="8">
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" s="2" customFormat="1" spans="1:2">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="1" spans="1:3">
       <c r="A24" s="8">
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" s="2" customFormat="1" spans="1:2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" s="2" customFormat="1" spans="1:3">
+      <c r="A25" s="8">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="26" s="2" customFormat="1" spans="1:2">
       <c r="A26" s="8"/>

</xml_diff>

<commit_message>
feat:update cowlevel and excel change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -116,7 +116,7 @@
     <t>Cowlevel001</t>
   </si>
   <si>
-    <t>506276.25|42784.48|46083.01||495329.25|43252.48|46083.01||497870.25|53525.48|46083.01||497870.25|53525.48|47007||503903.25|53525.48|47007||504647.25|47997.48|47007||499929.25|47997.48|47007</t>
+    <t>200239.58|99256.01|265.78||200851.58|99965.01|265.78||200738.58|101180.01|265.78||200609.58|100067.01|863.78</t>
   </si>
   <si>
     <t>Cowlevel002</t>
@@ -1067,7 +1067,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{8E19E395-D54C-409B-98D3-2393F0804047}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{BBCF855B-2181-4939-93EE-4D2B8714BBB9}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1076,7 +1076,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{E14272A0-B37D-4031-840A-CD97D57AD41B}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{A375437C-D222-4267-9F7B-98CF17ED6753}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1309,8 +1309,8 @@
   <sheetPr/>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" outlineLevelCol="5"/>
@@ -1533,7 +1533,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" s="2" customFormat="1" ht="33" spans="1:6">
+    <row r="19" s="2" customFormat="1" spans="1:6">
       <c r="A19" s="8">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
feat:update cow level excel change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -1144,7 +1144,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{CE68F97E-CA4C-49A7-9234-F5D54DE11700}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{22E3972C-2FB1-4295-86C4-1EB50C13316B}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1153,7 +1153,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{A8A50A9F-99D0-496F-9EB8-086F8B7DC791}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{23948ED1-7D83-4431-84CB-6B997447A43E}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1413,7 +1413,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
feat：update dragon excel and dragon point update
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="11925"/>
+    <workbookView windowWidth="24045" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>int</t>
   </si>
@@ -135,46 +135,25 @@
     <t>3006|-19105|1508</t>
   </si>
   <si>
-    <t>Cowlevel001</t>
-  </si>
-  <si>
-    <t>200239.58|99256.01|265.78||200851.58|99965.01|265.78||200738.58|101180.01|265.78||200609.58|100067.01|863.78</t>
-  </si>
-  <si>
-    <t>Cowlevel002</t>
-  </si>
-  <si>
-    <t>598563.75|594154.88|7143.97||602921.75|595009.88|7143.97||602921.75|595009.88|7851.97||602921.75|601241.88|7851.97||598241.75|602673.88|7851.97||598241.75|594819.88|7851.97||602921.75|600363.88|7295.97</t>
-  </si>
-  <si>
-    <t>Cowlevel003</t>
-  </si>
-  <si>
-    <t>498910.44|46868.74|45986||496482.44|48743.74|45986||498294.44|55570.74|45986||499992.44|56135.74|45986||499992.44|56135.74|46753.00||499228.44|47348.74|46753||496626.44|48303.74|46753||498189.44|55497.74|46424</t>
-  </si>
-  <si>
-    <t>Cowlevel004</t>
-  </si>
-  <si>
-    <t>97705.11|1001785.63|6204.8||97705.11|995826.63|6204.8||101330.11|995826.63|6204.8||101330.11|1001359.63|6204.80||101330.11|1001359.63|6911.80||97885.11|1001359.63|6911.80||97885.11|996353.63|6911.80||101778.11|996223.63|6911.80</t>
-  </si>
-  <si>
-    <t>Cowlevel005</t>
-  </si>
-  <si>
-    <t>98879.05|1000148.06|10082||98879.05|997982.06|10082||100784.05|997982.06|10082||100186.05|999942.06|10082||99185.45|999750.75|10589||99239.05|998549.06|10590||99851.05|998549.06|10590||99851.05|999709.06|10590</t>
-  </si>
-  <si>
-    <t>Cowlevel006</t>
-  </si>
-  <si>
-    <t>1010497.13|18739.56|4593.87||1006911.13|16723.56|4593.87||1004790.13|19763.56|4593.87||1006629.13|19763.56|5473.87||1009839.13|18905.56|5473.87||1007139.13|17599.56|5473.87</t>
-  </si>
-  <si>
-    <t>Cowlevel007</t>
-  </si>
-  <si>
-    <t>8978.4|229.39|296699.97||5201.4|229.39|296699.97||5201.4|5546.39|296699.97||6494.4|5546.39|296699.97||6494.4|5037.39|297305.97||6494.4|1696.39|297305.97||5428.4|3174.39|297305.97</t>
+    <t>赐福天光</t>
+  </si>
+  <si>
+    <t>火炎地狱</t>
+  </si>
+  <si>
+    <t>永眠之暗</t>
+  </si>
+  <si>
+    <t>天空树01</t>
+  </si>
+  <si>
+    <t>天空树02</t>
+  </si>
+  <si>
+    <t>荒野边疆</t>
+  </si>
+  <si>
+    <t>涌动之水</t>
   </si>
   <si>
     <t>Cowbirth001</t>
@@ -1147,7 +1126,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{9FC8BFB6-81E3-4081-85D6-927581E04C6D}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{76A1E481-49ED-4E07-9242-1C3410BCFF7F}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1156,7 +1135,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{F68B5EC7-8FDA-4C6A-A661-9EC51E6E7ACC}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{982EA6DB-75D9-40AE-BEBC-6948551D0688}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1416,7 +1395,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" outlineLevelCol="6"/>
@@ -1492,7 +1471,7 @@
       </c>
       <c r="C5" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B5,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>16</v>
@@ -1507,7 +1486,7 @@
       </c>
       <c r="C6" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B6,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>17</v>
@@ -1522,7 +1501,7 @@
       </c>
       <c r="C7" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B7,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>18</v>
@@ -1537,7 +1516,7 @@
       </c>
       <c r="C8" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B8,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>19</v>
@@ -1552,7 +1531,7 @@
       </c>
       <c r="C9" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B9,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>20</v>
@@ -1567,7 +1546,7 @@
       </c>
       <c r="C10" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B10,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>21</v>
@@ -1582,7 +1561,7 @@
       </c>
       <c r="C11" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B11,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>22</v>
@@ -1597,7 +1576,7 @@
       </c>
       <c r="C12" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B12,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>23</v>
@@ -1615,7 +1594,7 @@
       </c>
       <c r="C13" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B13,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>24</v>
@@ -1633,7 +1612,7 @@
       </c>
       <c r="C14" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B14,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>25</v>
@@ -1651,7 +1630,7 @@
       </c>
       <c r="C15" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B15,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>測試區域</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>26</v>
@@ -1669,7 +1648,7 @@
       </c>
       <c r="C16" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B16,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>龍吟村</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>28</v>
@@ -1687,7 +1666,7 @@
       </c>
       <c r="C17" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B17,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
+        <v>出生點</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>30</v>
@@ -1725,101 +1704,81 @@
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B19,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" s="3" customFormat="1" spans="1:4">
+    <row r="20" s="3" customFormat="1" spans="1:3">
       <c r="A20" s="10">
         <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B20,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" s="3" customFormat="1" spans="1:4">
+    </row>
+    <row r="21" s="3" customFormat="1" spans="1:3">
       <c r="A21" s="10">
         <v>17</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B21,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" s="3" customFormat="1" spans="1:4">
+    </row>
+    <row r="22" s="3" customFormat="1" spans="1:3">
       <c r="A22" s="10">
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B22,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" s="3" customFormat="1" spans="1:4">
+    </row>
+    <row r="23" s="3" customFormat="1" spans="1:3">
       <c r="A23" s="10">
         <v>19</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C23" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B23,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" s="3" customFormat="1" spans="1:4">
+    </row>
+    <row r="24" s="3" customFormat="1" spans="1:3">
       <c r="A24" s="10">
         <v>20</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C24" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B24,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" s="3" customFormat="1" spans="1:4">
+    </row>
+    <row r="25" s="3" customFormat="1" spans="1:3">
       <c r="A25" s="10">
         <v>21</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C25" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B25,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" spans="1:4">
@@ -1827,14 +1786,14 @@
         <v>22</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C26" s="7" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B26,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D26" s="11" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="1" spans="1:4">
@@ -1842,14 +1801,14 @@
         <v>23</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B27,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D27" s="11" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" s="3" customFormat="1" spans="1:4">
@@ -1857,14 +1816,14 @@
         <v>24</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C28" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B28,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D28" s="11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" s="3" customFormat="1" spans="1:4">
@@ -1872,14 +1831,14 @@
         <v>25</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B29,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D29" s="11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" s="3" customFormat="1" spans="1:4">
@@ -1887,14 +1846,14 @@
         <v>26</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C30" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B30,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D30" s="11" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" s="3" customFormat="1" spans="1:4">
@@ -1902,14 +1861,14 @@
         <v>27</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B31,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D31" s="11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" spans="1:4">
@@ -1917,14 +1876,14 @@
         <v>28</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C32" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B32,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D32" s="12" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1" spans="1:3">
@@ -1932,7 +1891,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C33" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B33,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
@@ -4774,7 +4733,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1">
         <v>2000</v>

</xml_diff>

<commit_message>
update：fog and delete fish level
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t xml:space="preserve">601881.5|-600237.8|-680.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cowbirth013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400174|99817|193</t>
   </si>
   <si>
     <t xml:space="preserve">Cowbirth014</t>
@@ -678,9 +672,9 @@
   <dimension ref="A1:G500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1518,19 +1512,9 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="n">
-        <v>55</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C59" s="1" t="str">
-        <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B59,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>93</v>
-      </c>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+      <c r="D59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="str">
@@ -4204,7 +4188,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="13" t="n">
         <v>2000</v>

</xml_diff>

<commit_message>
feat：update cowlevel new girl update
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="106">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -278,7 +278,7 @@
     <t xml:space="preserve">Cowbirth017</t>
   </si>
   <si>
-    <t xml:space="preserve">199422|97453|118</t>
+    <t xml:space="preserve">299389.4|196987|90.4</t>
   </si>
   <si>
     <t xml:space="preserve">Cowbirth018</t>
@@ -303,6 +303,45 @@
   </si>
   <si>
     <t xml:space="preserve">699229|204559|-351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">樱花森林</t>
+  </si>
+  <si>
+    <t xml:space="preserve">绿洲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河畔小巷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">覆潮之下</t>
+  </si>
+  <si>
+    <t xml:space="preserve">糖果乐园</t>
+  </si>
+  <si>
+    <t xml:space="preserve">巫师豪宅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">观测站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">很喜欢的宇宙阴暗场景</t>
+  </si>
+  <si>
+    <t xml:space="preserve">温泉旅馆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">寻常一角</t>
+  </si>
+  <si>
+    <t xml:space="preserve">洞穴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">炼狱城堡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高塔</t>
   </si>
   <si>
     <t xml:space="preserve">MaxLanItemCount</t>
@@ -672,9 +711,9 @@
   <dimension ref="A1:G500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
+      <selection pane="bottomLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1512,77 +1551,153 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0"/>
-      <c r="C59" s="0"/>
-      <c r="D59" s="0"/>
+      <c r="A59" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="C60" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B60,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="C61" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B61,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="C62" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B62,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="C63" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B63,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="C64" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B64,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="C65" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B65,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C66" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B66,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="C67" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B67,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="C68" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B68,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C69" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B69,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="C70" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B70,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="C71" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B71,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -4188,7 +4303,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B1" s="13" t="n">
         <v>2000</v>

</xml_diff>

<commit_message>
feat：update some bug fix
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -711,9 +711,9 @@
   <dimension ref="A1:G500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="2" t="n">
         <v>55</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -1560,7 +1560,7 @@
       <c r="C59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
+      <c r="A60" s="2" t="n">
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="2" t="n">
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="2" t="n">
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1596,7 +1596,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="2" t="n">
         <v>59</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1608,7 +1608,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="2" t="n">
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1620,7 +1620,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="2" t="n">
         <v>61</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
+      <c r="A66" s="2" t="n">
         <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+      <c r="A67" s="2" t="n">
         <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1656,7 +1656,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+      <c r="A68" s="2" t="n">
         <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -1668,7 +1668,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+      <c r="A69" s="2" t="n">
         <v>65</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1680,7 +1680,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
+      <c r="A70" s="2" t="n">
         <v>66</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1692,7 +1692,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+      <c r="A71" s="2" t="n">
         <v>67</v>
       </c>
       <c r="B71" s="1" t="s">

</xml_diff>

<commit_message>
fix:water cow level ai walk
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -149,7 +149,7 @@
     <t xml:space="preserve">Cowbirth001</t>
   </si>
   <si>
-    <t xml:space="preserve">7983.23|1689.94|297205.16</t>
+    <t xml:space="preserve">137194|-55195.01|-1771</t>
   </si>
   <si>
     <t xml:space="preserve">Cowbirth002</t>
@@ -711,9 +711,9 @@
   <dimension ref="A1:G500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
+      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat:update new birth point
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -122,7 +122,7 @@
     <t xml:space="preserve">BirthPoint</t>
   </si>
   <si>
-    <t xml:space="preserve">3006|-19105|1508</t>
+    <t xml:space="preserve">3006|-19105|1508||3213.64|-19445.52|1507.5||3393.64|-19445.52|1507.50||3619.64|-19445.52|1507.50||3870.64|-19445.52|1507.50||4094.64|-19445.52|1507.50||4270.64|-19445.52|1507.50||4505.64|-19445.52|1507.50||4505.64|-19181.52|1507.50||4276.64|-19181.52|1507.50||4081.64|-19181.52|1507.50||3849.64|-19181.52|1507.50||3640.64|-19181.52|1507.50||3420.64|-19181.52|1507.50||3220.64|-19181.52|1507.50||3006.64|-19181.52|1507.50||3006.64|-18867.52|1507.50||3215.64|-18867.52|1507.50||3494.64|-18867.52|1507.50||3702.64|-18867.52|1507.50||3914.64|-18867.52|1507.50||4127.64|-18867.52|1507.50||4326.64|-18867.52|1507.50||4504.64|-18867.52|1507.50||4504.64|-19862.52|1507.50||4242.64|-19862.52|1507.50||4024.64|-19862.52|1507.50||3824.64|-19862.52|1507.50||3592.64|-19862.52|1507.50||3363.64|-19862.52|1507.50||3219.64|-19862.52|1507.50||3061.64|-19862.52|1507.50</t>
   </si>
   <si>
     <t xml:space="preserve">赐福天光</t>
@@ -713,7 +713,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -988,7 +988,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="1" customFormat="true" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
feat：update area excel change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -122,7 +122,7 @@
     <t xml:space="preserve">BirthPoint</t>
   </si>
   <si>
-    <t xml:space="preserve">3006|-19105|1508||3213.64|-19445.52|1507.5||3393.64|-19445.52|1507.50||3619.64|-19445.52|1507.50||3870.64|-19445.52|1507.50||4094.64|-19445.52|1507.50||4270.64|-19445.52|1507.50||4505.64|-19445.52|1507.50||4505.64|-19181.52|1507.50||4276.64|-19181.52|1507.50||4081.64|-19181.52|1507.50||3849.64|-19181.52|1507.50||3640.64|-19181.52|1507.50||3420.64|-19181.52|1507.50||3220.64|-19181.52|1507.50||3006.64|-19181.52|1507.50||3006.64|-18867.52|1507.50||3215.64|-18867.52|1507.50||3494.64|-18867.52|1507.50||3702.64|-18867.52|1507.50||3914.64|-18867.52|1507.50||4127.64|-18867.52|1507.50||4326.64|-18867.52|1507.50||4504.64|-18867.52|1507.50||4504.64|-19862.52|1507.50||4242.64|-19862.52|1507.50||4024.64|-19862.52|1507.50||3824.64|-19862.52|1507.50||3592.64|-19862.52|1507.50||3363.64|-19862.52|1507.50||3219.64|-19862.52|1507.50||3061.64|-19862.52|1507.50</t>
+    <t xml:space="preserve">3006|-19105|1508||3213.64|-19445.52|1507.5||3393.64|-19445.52|1507.50||3619.64|-19445.52|1507.50||3870.64|-19445.52|1507.50||4094.64|-19445.52|1507.50||4270.64|-19445.52|1507.50||4505.64|-19445.52|1507.50||4505.64|-19181.52|1507.50||4276.64|-19181.52|1507.50||4081.64|-19181.52|1507.50||3640.64|-19181.52|1507.50||3420.64|-19181.52|1507.50||3220.64|-19181.52|1507.50||3006.64|-19181.52|1507.50||3006.64|-18867.52|1507.50||3215.64|-18867.52|1507.50||3494.64|-18867.52|1507.50||3702.64|-18867.52|1507.50||3914.64|-18867.52|1507.50||4127.64|-18867.52|1507.50||4326.64|-18867.52|1507.50||4504.64|-18867.52|1507.50||4504.64|-19862.52|1507.50||4242.64|-19862.52|1507.50||4024.64|-19862.52|1507.50||3824.64|-19862.52|1507.50||3592.64|-19862.52|1507.50||3363.64|-19862.52|1507.50||3219.64|-19862.52|1507.50||3061.64|-19862.52|1507.50</t>
   </si>
   <si>
     <t xml:space="preserve">赐福天光</t>
@@ -713,7 +713,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat：update new cow level
剩余6个有问题的预制体奶牛关场景
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="124">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -348,6 +348,54 @@
   </si>
   <si>
     <t xml:space="preserve">701524|300346|8381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">神秘传送门</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700000|402615|1979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天穹之上</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700000|498353|770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林中深处</t>
+  </si>
+  <si>
+    <t xml:space="preserve">701258|703009|832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">龙娘洞窟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">601088|708812|3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">木灵宫殿</t>
+  </si>
+  <si>
+    <t xml:space="preserve">507563|599962|76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水之城都</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399854|599086|1080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陵墓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399727.5|70245|21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">幽灵城</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500000|700300|49</t>
   </si>
   <si>
     <t xml:space="preserve">MaxLanItemCount</t>
@@ -361,7 +409,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -400,6 +448,13 @@
       <name val="微软雅黑"/>
       <family val="0"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -523,8 +578,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -807,9 +862,9 @@
   <dimension ref="A1:G500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D72" activeCellId="0" sqref="D72"/>
+      <selection pane="bottomLeft" activeCell="C81" activeCellId="0" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1466,7 +1521,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" s="18" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="17" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="n">
         <v>43</v>
       </c>
@@ -1480,7 +1535,6 @@
       <c r="D47" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="17"/>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="n">
@@ -1572,7 +1626,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" s="18" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="17" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="n">
         <v>50</v>
       </c>
@@ -1586,7 +1640,6 @@
       <c r="D54" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E54" s="17"/>
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="n">
@@ -1802,7 +1855,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
+      <c r="A72" s="2" t="n">
         <v>68</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -1817,51 +1870,123 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C73" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B73,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D73" s="15" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="C74" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B74,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D74" s="15" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="C75" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B75,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D75" s="15" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="C76" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B76,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D76" s="15" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>115</v>
+      </c>
       <c r="C77" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B77,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D77" s="15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="C78" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B78,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D78" s="15" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="C79" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B79,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D79" s="15" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="C80" s="1" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B80,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4535,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B1" s="19" t="n">
         <v>2000</v>

</xml_diff>

<commit_message>
feat：fix cowlevel back birthpoint
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Area_区域表.xlsx
+++ b/dragon-verse/Excels/Area_区域表.xlsx
@@ -122,7 +122,7 @@
     <t xml:space="preserve">BirthPoint</t>
   </si>
   <si>
-    <t xml:space="preserve">3006|-19105|1508||3213.64|-19445.52|1507.5||3393.64|-19445.52|1507.50||3619.64|-19445.52|1507.50||3870.64|-19445.52|1507.50||4094.64|-19445.52|1507.50||4270.64|-19445.52|1507.50||4505.64|-19445.52|1507.50||4505.64|-19181.52|1507.50||4276.64|-19181.52|1507.50||4081.64|-19181.52|1507.50||3640.64|-19181.52|1507.50||3420.64|-19181.52|1507.50||3220.64|-19181.52|1507.50||3006.64|-19181.52|1507.50||3006.64|-18867.52|1507.50||3215.64|-18867.52|1507.50||3494.64|-18867.52|1507.50||3702.64|-18867.52|1507.50||3914.64|-18867.52|1507.50||4127.64|-18867.52|1507.50||4326.64|-18867.52|1507.50||4504.64|-18867.52|1507.50||4504.64|-19862.52|1507.50||4242.64|-19862.52|1507.50||4024.64|-19862.52|1507.50||3824.64|-19862.52|1507.50||3592.64|-19862.52|1507.50||3363.64|-19862.52|1507.50||3219.64|-19862.52|1507.50||3061.64|-19862.52|1507.50</t>
+    <t xml:space="preserve">-3076|-6842|1085.5||-2869.36|-6841.52|1085.5||-2689.36|-6841.52|1085.5||-2463.36|-6841.52|1085.5||-2216.36|-6841.52|1085.5||-1988.36|-6841.52|1085.5||-1812.36|-6841.52|1085.5||-1577.36|-6841.52|1085.5||-1577.36|-6577.52|1085.50||-1806.36|-6577.52|1085.50||-2001.36|-65577.52|1085.50||-2233.36|-6577.52|1085.50||-2442.36|-6577.52|1085.50||-2662.36|-6577.52|1085.50||-2862.36|-6577.52|1085.50||-3076.36|-6577.52|1085.50||-3076.36|-6263.52|1085.50||-2867.36|-6263.52|1085.50||-2588.36|-6263.52|1085.50||-2380.36|-6263.52|1085.50||-2168.36|-6263.52|1085.50||-1955.36|-6263.52|1085.50||-1756.36|-6263.52|1085.50||-1578.36|-6263.52|1085.50||-1578.36|-7258.52|1085.50||-1840.36|-7258.52|1085.50||-2058.36|-7258.52|1085.50||-2258.36|-7258.52|1085.50||-2490.36|-7258.52|1085.50||-2719.36|-7258.52|1085.50||-2863.36|-7258.52|1085.50||-3021.36|-7258.52|1085.50</t>
   </si>
   <si>
     <t xml:space="preserve">赐福天光</t>
@@ -889,9 +889,9 @@
   <dimension ref="A1:G501"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D98" activeCellId="0" sqref="D98"/>
+      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>